<commit_message>
Mars Project SpecFlow Task
</commit_message>
<xml_diff>
--- a/mars.specflow-master/SpecflowPages/Files/TestDataShareSkill.xlsx
+++ b/mars.specflow-master/SpecflowPages/Files/TestDataShareSkill.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="9870"/>
+    <workbookView windowWidth="15910" windowHeight="9760"/>
   </bookViews>
   <sheets>
     <sheet name="ShareSkill" sheetId="2" r:id="rId1"/>
@@ -168,13 +168,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="178" formatCode="hh:mm:ss;@"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -204,6 +204,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -211,8 +226,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,13 +236,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,11 +255,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -263,10 +272,56 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -278,34 +333,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -315,37 +346,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -368,181 +368,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,6 +608,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -619,15 +634,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,8 +656,19 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -682,26 +699,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -711,10 +711,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -723,134 +723,134 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1255,7 +1255,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1355,10 +1355,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="5">
-        <v>44341</v>
+        <v>44365</v>
       </c>
       <c r="I2" s="5">
-        <v>44465</v>
+        <v>44764</v>
       </c>
       <c r="J2" s="13">
         <v>1</v>

</xml_diff>